<commit_message>
Error instead of Infinity from division by 0
</commit_message>
<xml_diff>
--- a/tests/Manual Testing Log.xlsx
+++ b/tests/Manual Testing Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dalla\quic-calc\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3233862-BC70-45AD-B1F6-C99333C59A24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53248037-5B68-48D3-AC74-0631AD342EAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2472" windowWidth="23040" windowHeight="12204" xr2:uid="{ACA48E57-C6D3-4A0F-B3D5-E187FCCD8CE2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{ACA48E57-C6D3-4A0F-B3D5-E187FCCD8CE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Testing Log" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="56">
   <si>
     <t>Date</t>
   </si>
@@ -92,9 +92,6 @@
     <t>[Backspace] result of 12 from: 123, enter backspace</t>
   </si>
   <si>
-    <t>[Divide by Zero] result of Infinity from: 7 / 0</t>
-  </si>
-  <si>
     <t>[Formatting] result shows "1,234,567.89" from: 1234567.89</t>
   </si>
   <si>
@@ -140,9 +137,6 @@
     <t>[Backspace] result of 0 from: 52, backspace, backspace</t>
   </si>
   <si>
-    <t>[Negative] equation does NOT contain "Infinity" from: 2 / 0 =, +</t>
-  </si>
-  <si>
     <t>[Large Num Error] result shows "Too Much!" from: 9, square, square, square, square</t>
   </si>
   <si>
@@ -206,9 +200,6 @@
     <t>[Exponent] result of -216 from: -6 ^ 3</t>
   </si>
   <si>
-    <t>[Backspace] result shows "-" from: -55, backspace, backspace</t>
-  </si>
-  <si>
     <t>[Negative] result shows 23 from: 023</t>
   </si>
   <si>
@@ -216,6 +207,18 @@
   </si>
   <si>
     <t>[Exponent] result of 0.04 from: 25 ^ -1</t>
+  </si>
+  <si>
+    <t>2020-30-09</t>
+  </si>
+  <si>
+    <t>[Divide By Zero] "Cannot Divide By Zero" result from: 9 / 0</t>
+  </si>
+  <si>
+    <t>[Divide By Zero] "Cannot Divide By Zero" result from: 12 * 8 / 0</t>
+  </si>
+  <si>
+    <t>[Backspace] result shows "0" from: -55, backspace, backspace</t>
   </si>
 </sst>
 </file>
@@ -600,7 +603,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -631,101 +634,101 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -733,404 +736,404 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
         <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
         <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
         <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
         <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B22" t="s">
         <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B23" t="s">
         <v>30</v>
       </c>
       <c r="C23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B24" t="s">
         <v>31</v>
       </c>
       <c r="C24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B25" t="s">
         <v>32</v>
       </c>
       <c r="C25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B26" t="s">
         <v>33</v>
       </c>
       <c r="C26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="B27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B29" t="s">
         <v>37</v>
       </c>
       <c r="C29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B30" t="s">
         <v>38</v>
       </c>
       <c r="C30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B31" t="s">
         <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B32" t="s">
         <v>40</v>
       </c>
       <c r="C32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B33" t="s">
         <v>41</v>
       </c>
       <c r="C33" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B34" t="s">
         <v>42</v>
       </c>
       <c r="C34" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>43</v>
       </c>
       <c r="C35" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B36" t="s">
         <v>44</v>
       </c>
       <c r="C36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B37" t="s">
         <v>45</v>
       </c>
       <c r="C37" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B38" t="s">
         <v>46</v>
       </c>
       <c r="C38" t="s">
-        <v>18</v>
+        <v>21</v>
+      </c>
+      <c r="D38">
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B39" t="s">
         <v>47</v>
       </c>
       <c r="C39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B40" t="s">
         <v>48</v>
       </c>
       <c r="C40" t="s">
-        <v>22</v>
-      </c>
-      <c r="D40">
-        <v>3</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B41" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C41" t="s">
-        <v>18</v>
+        <v>21</v>
+      </c>
+      <c r="D41">
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B42" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C42" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C43" t="s">
-        <v>22</v>
-      </c>
-      <c r="D43">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C44" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="B45" t="s">
         <v>53</v>
       </c>
       <c r="C45" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="B46" t="s">
         <v>54</v>
       </c>
       <c r="C46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>